<commit_message>
update Excel and API import processes
</commit_message>
<xml_diff>
--- a/static/file/import_product_migrations_template.xlsx
+++ b/static/file/import_product_migrations_template.xlsx
@@ -1,20 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="27610"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="11110"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hoelsner/Projects/coding-projects-on-github/product-database/src/source/static/file/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hoelsner/Projects/github-projects/product-database/src/source/static/file/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B73CA87-1970-1F4B-A1A7-B0FB788E7D20}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="20460" tabRatio="500"/>
+    <workbookView xWindow="16800" yWindow="460" windowWidth="16800" windowHeight="20540" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="product_migrations" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="140000" concurrentCalc="0"/>
+  <calcPr calcId="140000"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
@@ -26,8 +27,43 @@
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>Henry Ölsner</author>
+  </authors>
+  <commentList>
+    <comment ref="B1" authorId="0" shapeId="0" xr:uid="{A90CC075-E58A-5D49-B9F1-991EF3346E2A}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">"Cisco Systems"
+</t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t>"Juniper Networks"</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
     <t>Product ID</t>
   </si>
@@ -43,12 +79,15 @@
   <si>
     <t>Migration Product Info URL</t>
   </si>
+  <si>
+    <t>Vendor</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="4" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -79,6 +118,13 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -129,6 +175,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -455,41 +504,45 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:F1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomRight" activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="30.83203125" customWidth="1"/>
-    <col min="2" max="5" width="35.5" customWidth="1"/>
+    <col min="1" max="2" width="30.83203125" customWidth="1"/>
+    <col min="3" max="6" width="35.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="2" customFormat="1" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" s="2" customFormat="1" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>4</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <legacyDrawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>